<commit_message>
code updated with multiple client execution
</commit_message>
<xml_diff>
--- a/testdata/clientTestData/Bluegreen.xlsx
+++ b/testdata/clientTestData/Bluegreen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Documents/RallyMochaFramework/testdata/clientTestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F6CC0D-A92C-A942-95ED-C5BE74C1B022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607693E6-2C7C-F846-9498-288E8843C1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>